<commit_message>
change dashboard page, add table page, add downloads page, add option to merging tables with custom colums
</commit_message>
<xml_diff>
--- a/admin/Assets/files/table.xlsx
+++ b/admin/Assets/files/table.xlsx
@@ -15,33 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
   <si>
     <t>id</t>
-  </si>
-  <si>
-    <t>date_reg</t>
-  </si>
-  <si>
-    <t>2018-10-15 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-11-05 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-05-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2018-01-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-10-14 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-01-22 00:00:00</t>
-  </si>
-  <si>
-    <t>2017-12-20 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -380,7 +356,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -388,68 +364,665 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>99</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>98</v>
+      </c>
+      <c r="C4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>97</v>
+      </c>
+      <c r="C5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>96</v>
+      </c>
+      <c r="C6">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>95</v>
+      </c>
+      <c r="C7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>94</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>92</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>91</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>90</v>
+      </c>
+      <c r="C12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>89</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>88</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>87</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>86</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>85</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>84</v>
+      </c>
+      <c r="C18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>83</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>82</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
+      <c r="B21">
+        <v>81</v>
+      </c>
+      <c r="C21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22">
+        <v>80</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23">
+        <v>79</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24">
+        <v>78</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25">
+        <v>77</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26">
+        <v>76</v>
+      </c>
+      <c r="C26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27">
+        <v>75</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="B28">
+        <v>74</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="B29">
+        <v>73</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30">
+        <v>72</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="B31">
+        <v>71</v>
+      </c>
+      <c r="C31">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="32" spans="1:3">
+      <c r="B32">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="B33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="B34">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="B35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="B36">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="B37">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="B38">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="B39">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="B40">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="B41">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="B42">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="B43">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="B46">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="B47">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="B48">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="B49">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="B53">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="B54">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="B56">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="B57">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="B59">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="B60">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="B61">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="B62">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="B63">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="B64">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="B65">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="B66">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="B67">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="B68">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="B69">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="B70">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="B71">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="B72">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="B73">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="B74">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="B75">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="B76">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="B77">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="B78">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="B79">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="B80">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="B81">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="B82">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="B83">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="B84">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="B85">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="B86">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="B87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="B88">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="B89">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="B90">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="B91">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="B92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="B93">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="B94">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="B95">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="B96">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="B97">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="B98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="B99">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="B100">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
+    <row r="101" spans="1:3">
+      <c r="B101">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>